<commit_message>
Finished the Shot list
</commit_message>
<xml_diff>
--- a/ShotList.xlsx
+++ b/ShotList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0668625\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0668625\Desktop\Indianamation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="109">
   <si>
     <t>Shot #</t>
   </si>
@@ -302,13 +302,55 @@
     <t>front view of the car as the explosion approaches and eventually engulfs it, pushing it towards the screen</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=vxkamWaya8k</t>
-  </si>
-  <si>
-    <t>Start at about 2:20</t>
-  </si>
-  <si>
     <t>Stop about 3:08</t>
+  </si>
+  <si>
+    <t>ES/LS</t>
+  </si>
+  <si>
+    <t>Crane down and back</t>
+  </si>
+  <si>
+    <t>Fridge</t>
+  </si>
+  <si>
+    <t>fridge flies in from the distance above, bounces and creates a dust cloud, then flies off screen</t>
+  </si>
+  <si>
+    <t>fridge bounces down a hill from right to left</t>
+  </si>
+  <si>
+    <t>fridge bounces down hill, away from camera</t>
+  </si>
+  <si>
+    <t>LS, LA</t>
+  </si>
+  <si>
+    <t>fridge bounces down hill, towards camer. Comes to a stop and Indy rolls out</t>
+  </si>
+  <si>
+    <t>Indy finishes roll, catches breath and looks forward</t>
+  </si>
+  <si>
+    <t>MS, OTS</t>
+  </si>
+  <si>
+    <t>Indy, Gopher</t>
+  </si>
+  <si>
+    <t>Indy spots gopher. Gopher drops his snack and scurries into hole, while Indy stands up and walks off</t>
+  </si>
+  <si>
+    <t>MS/ES</t>
+  </si>
+  <si>
+    <t>Indy, Nucluer explosion</t>
+  </si>
+  <si>
+    <t>Cranes with Indy</t>
+  </si>
+  <si>
+    <t>Indy walks up hill as a giant flash happens. He looks on as the mushroom cloud envelops the sky</t>
   </si>
 </sst>
 </file>
@@ -397,10 +439,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -752,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:D30"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -769,18 +811,18 @@
     <col min="7" max="7" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -802,11 +844,11 @@
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -828,14 +870,14 @@
       <c r="G3" t="s">
         <v>37</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -857,14 +899,14 @@
       <c r="G4" t="s">
         <v>39</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>10</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -886,14 +928,14 @@
       <c r="G5" t="s">
         <v>43</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>12</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -915,14 +957,14 @@
       <c r="G6" t="s">
         <v>47</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>14</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -944,14 +986,14 @@
       <c r="G7" t="s">
         <v>50</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>16</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -973,14 +1015,14 @@
       <c r="G8" t="s">
         <v>52</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>18</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1002,14 +1044,14 @@
       <c r="G9" t="s">
         <v>79</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>20</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1031,14 +1073,14 @@
       <c r="G10" t="s">
         <v>58</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>22</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1060,14 +1102,14 @@
       <c r="G11" t="s">
         <v>60</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>24</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1089,14 +1131,14 @@
       <c r="G12" t="s">
         <v>62</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>26</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1119,7 +1161,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1145,7 +1187,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1171,7 +1213,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1459,19 +1501,170 @@
         <v>91</v>
       </c>
     </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" t="s">
+        <v>95</v>
+      </c>
+      <c r="G29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" t="s">
+        <v>95</v>
+      </c>
+      <c r="G30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2">
+        <v>6.2499999999999995E-3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>8</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>